<commit_message>
add in new covariates - pollock recruitment
gets added into stage a.
- remove zooplankton because it is positively correlated with temperature
hmm age comps gets worse just changing the covariate??
- changed how pollock was mean scaled so ti was just the yeras in model
- added in size, havent run yet just tidied
</commit_message>
<xml_diff>
--- a/AYK Covariates Table.xlsx
+++ b/AYK Covariates Table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/genoasullaway/Documents/GitHub/AYK_prey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232BF3B1-8DA9-AB43-A169-80310AD7F344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CA95FB-45DA-A546-A248-DE31B5C7E9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4060" yWindow="760" windowWidth="26880" windowHeight="19140" xr2:uid="{15635B22-154F-5C4D-8D09-E55D0FC35932}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>Stage</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t xml:space="preserve">maybe greg R has updated wild fish abundances too post pub - check. </t>
+  </si>
+  <si>
+    <t>added 10-30-24</t>
   </si>
 </sst>
 </file>
@@ -567,7 +570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -641,9 +644,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -662,6 +662,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -670,9 +673,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1011,7 +1011,7 @@
   <dimension ref="B1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1065,8 +1065,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="26"/>
+      <c r="I2" s="25"/>
     </row>
     <row r="3" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
@@ -1085,8 +1084,7 @@
         <v>14</v>
       </c>
       <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="26"/>
+      <c r="I3" s="25"/>
     </row>
     <row r="4" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
@@ -1105,8 +1103,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="26"/>
+      <c r="I4" s="25"/>
     </row>
     <row r="5" spans="2:9" ht="68" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
@@ -1127,10 +1124,10 @@
       <c r="G5" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="26"/>
+      <c r="I5" s="25"/>
     </row>
     <row r="6" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
@@ -1151,8 +1148,10 @@
       <c r="G6" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26"/>
+      <c r="H6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="25"/>
     </row>
     <row r="7" spans="2:9" ht="120" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
@@ -1173,10 +1172,10 @@
       <c r="G7" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="27" t="s">
+      <c r="I7" s="26" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1199,8 +1198,7 @@
       <c r="G8" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="26"/>
+      <c r="I8" s="25"/>
     </row>
     <row r="9" spans="2:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
@@ -1221,8 +1219,7 @@
       <c r="G9" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="25"/>
-      <c r="I9" s="26"/>
+      <c r="I9" s="25"/>
     </row>
     <row r="10" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
@@ -1241,8 +1238,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="24"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="26"/>
+      <c r="I10" s="25"/>
     </row>
     <row r="11" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="s">
@@ -1263,11 +1259,10 @@
       <c r="G11" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="25"/>
-      <c r="I11" s="26"/>
+      <c r="I11" s="25"/>
     </row>
     <row r="12" spans="2:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="30" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -1282,13 +1277,13 @@
       <c r="F12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="G12" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="29" t="s">
+      <c r="H12" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="I12" s="30"/>
+      <c r="I12" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
doing a little better - now estimating sigma juveniles
- theta signal is getting swamped though.
- gonna adjust priors, and estimate sigma brood year return too
-mess with sigma priors a bit
</commit_message>
<xml_diff>
--- a/AYK Covariates Table.xlsx
+++ b/AYK Covariates Table.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/genoasullaway/Documents/GitHub/AYK_prey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CA95FB-45DA-A546-A248-DE31B5C7E9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1098DB-0149-E349-A006-D4D90868DC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4060" yWindow="760" windowWidth="26880" windowHeight="19140" xr2:uid="{15635B22-154F-5C4D-8D09-E55D0FC35932}"/>
+    <workbookView xWindow="34560" yWindow="500" windowWidth="36560" windowHeight="21100" xr2:uid="{15635B22-154F-5C4D-8D09-E55D0FC35932}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table 1 Covariates" sheetId="3" r:id="rId1"/>
+    <sheet name="Table 2 Priors" sheetId="4" r:id="rId2"/>
+    <sheet name="Supplement covariate data links" sheetId="5" r:id="rId3"/>
+    <sheet name="Old covariate table with tested" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="76">
   <si>
     <t>Stage</t>
   </si>
@@ -174,13 +177,122 @@
   </si>
   <si>
     <t>added 10-30-24</t>
+  </si>
+  <si>
+    <t>Lag from brood year (t)</t>
+  </si>
+  <si>
+    <t>Covariate Name</t>
+  </si>
+  <si>
+    <t>Covariate Data Source</t>
+  </si>
+  <si>
+    <t>Citations</t>
+  </si>
+  <si>
+    <t>Proposed Mechanism</t>
+  </si>
+  <si>
+    <t>Feddern et al 2024, Ohlberger et al 2020</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Caption</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+  </si>
+  <si>
+    <t>Table 1: Table of covariates used in the life cycle model, associated stage, lag from the brood year, hypothesis and citations. See supplement for links to all publically available covariate data sources</t>
+  </si>
+  <si>
+    <t>ADFG ASL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://nwis.waterdata.usgs.gov/nwis/inventory/?site_no=15565447</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YUKON DISCHARGE </t>
+  </si>
+  <si>
+    <t>pollock</t>
+  </si>
+  <si>
+    <t>https://apps-afsc.fisheries.noaa.gov/Plan_Team/2023/EBSPollock.pdf</t>
+  </si>
+  <si>
+    <t>chum hatchery</t>
+  </si>
+  <si>
+    <t>pink harchery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.npafc.org/statistics/ </t>
+  </si>
+  <si>
+    <t>NBS SST</t>
+  </si>
+  <si>
+    <t>https://shinyfin.psmfc.org/</t>
+  </si>
+  <si>
+    <t>Aleutian SST</t>
+  </si>
+  <si>
+    <t>Fullness index</t>
+  </si>
+  <si>
+    <t>[check about publically avail??]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NBS Cummulative Degree Days </t>
+  </si>
+  <si>
+    <t>Pollock Recruitment Index</t>
+  </si>
+  <si>
+    <t>Ianelli J, Honkalehto T, Wassermann S, Lauffenburger N, McGilliard C, Siddon E (2023) Stock assessment for eastern Bering Sea walleye pollock. North Pacific Fishery Management Council, Anchorage, AK.</t>
+  </si>
+  <si>
+    <t>t+2</t>
+  </si>
+  <si>
+    <t>North Pacific Anadromous Fish Commission</t>
+  </si>
+  <si>
+    <t>AKFIN</t>
+  </si>
+  <si>
+    <t>Time Series</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mean  E Aleutian SST summed November - March</t>
+  </si>
+  <si>
+    <t>Sea surface</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -202,16 +314,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -566,11 +696,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -672,6 +817,47 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1007,10 +1193,347 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C922C39-C49D-8D4D-BCBE-7247337ED328}">
+  <dimension ref="B1:I15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="167" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="4"/>
+    <col min="3" max="3" width="40.83203125" style="4" customWidth="1"/>
+    <col min="4" max="6" width="32.83203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="4"/>
+    <col min="8" max="8" width="20.5" style="4" customWidth="1"/>
+    <col min="9" max="9" width="24" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="49" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B2" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+    </row>
+    <row r="3" spans="2:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="B3" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="41"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+    </row>
+    <row r="4" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B4" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+    </row>
+    <row r="5" spans="2:9" ht="137" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+    </row>
+    <row r="7" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B7" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="40"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46">
+        <v>0</v>
+      </c>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+    </row>
+    <row r="8" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B8" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="46"/>
+    </row>
+    <row r="9" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+    </row>
+    <row r="14" spans="2:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="C14" s="36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="C15" s="35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6D1E8C-B800-DB41-95B4-3695A974BBA7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D78B096-5A74-CC44-8B21-3349AED14402}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="64.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="78" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="37"/>
+      <c r="B9" s="37"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="37"/>
+      <c r="B10" s="37"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="37"/>
+      <c r="B12" s="37"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="37"/>
+      <c r="B13" s="37"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="37"/>
+      <c r="B14" s="37"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{084D3D18-8C71-464C-A320-63E682CA5315}">
   <dimension ref="B1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="65" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>

</xml_diff>